<commit_message>
check: test can be submitted only once by an individual
</commit_message>
<xml_diff>
--- a/Backend/Data/AccountData/accounts.xlsx
+++ b/Backend/Data/AccountData/accounts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WEB PROJECTS\TreasureHuntTestConductor\Backend\Data\AccountData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF41F8CB-1B71-4DCD-BB50-4890AE9D3519}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A1A6063-EDBB-4723-B00B-BF2B8F2ECD92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3696" yWindow="3360" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -429,7 +429,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
total question count set to 10
</commit_message>
<xml_diff>
--- a/Backend/Data/AccountData/accounts.xlsx
+++ b/Backend/Data/AccountData/accounts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WEB PROJECTS\TreasureHuntTestConductor\Backend\Data\AccountData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A1A6063-EDBB-4723-B00B-BF2B8F2ECD92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC45BFC4-F5E9-4A46-87B9-015EB2B065D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3696" yWindow="3360" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
   <si>
     <t>Madhukrishna Nipankar</t>
   </si>
@@ -67,44 +67,17 @@
     <t>lastName</t>
   </si>
   <si>
-    <t>alajlksdjas</t>
-  </si>
-  <si>
-    <t>sdasd</t>
-  </si>
-  <si>
-    <t>dsad</t>
-  </si>
-  <si>
-    <t>asdasd</t>
-  </si>
-  <si>
     <t>password</t>
   </si>
   <si>
-    <t>Yadnesh Gangurde</t>
-  </si>
-  <si>
-    <t>gangurde.yadnesh22@pict.org</t>
-  </si>
-  <si>
-    <t>Rajesh Phursule</t>
-  </si>
-  <si>
-    <t>rajesh.phursule22@pict.org</t>
-  </si>
-  <si>
-    <t>Daman Parja</t>
-  </si>
-  <si>
-    <t>daman.parja@pict.org</t>
+    <t>Pccoe</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -119,6 +92,16 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -138,17 +121,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="2" xr:uid="{8AB50278-1F4D-4632-B8B1-C3A1F5AF63EF}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -426,15 +413,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D87"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.21875" customWidth="1"/>
+    <col min="1" max="1" width="40.21875" customWidth="1"/>
     <col min="2" max="2" width="48.5546875" customWidth="1"/>
     <col min="3" max="3" width="20.33203125" customWidth="1"/>
   </cols>
@@ -447,7 +434,7 @@
         <v>11</v>
       </c>
       <c r="C1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D1" t="s">
         <v>12</v>
@@ -464,7 +451,7 @@
         <v>9518311216</v>
       </c>
       <c r="D2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -492,7 +479,7 @@
         <v>9356062932</v>
       </c>
       <c r="D4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -506,7 +493,7 @@
         <v>1321313123</v>
       </c>
       <c r="D5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -520,50 +507,407 @@
         <v>2221323133</v>
       </c>
       <c r="D6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7">
-        <v>1111111111</v>
-      </c>
-      <c r="D7" t="s">
-        <v>16</v>
-      </c>
+      <c r="B7" s="1"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8">
-        <v>2222222222</v>
-      </c>
-      <c r="D8" t="s">
-        <v>16</v>
-      </c>
+      <c r="B8" s="1"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C9">
-        <v>3333333333</v>
-      </c>
-      <c r="D9" t="s">
-        <v>16</v>
-      </c>
+      <c r="B9" s="1"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="3"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="3"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="3"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="3"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="3"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="3"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="3"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="3"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="3"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="2"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="3"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="2"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="3"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="3"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="2"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="3"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="2"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="3"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="2"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="3"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="2"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="3"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="2"/>
+      <c r="B26" s="2"/>
+      <c r="C26" s="3"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="2"/>
+      <c r="B27" s="2"/>
+      <c r="C27" s="3"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" s="2"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="3"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" s="2"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="3"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" s="2"/>
+      <c r="B30" s="2"/>
+      <c r="C30" s="3"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" s="2"/>
+      <c r="B31" s="2"/>
+      <c r="C31" s="3"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" s="2"/>
+      <c r="B32" s="2"/>
+      <c r="C32" s="3"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" s="2"/>
+      <c r="B33" s="2"/>
+      <c r="C33" s="3"/>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" s="2"/>
+      <c r="B34" s="2"/>
+      <c r="C34" s="3"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" s="2"/>
+      <c r="B35" s="2"/>
+      <c r="C35" s="3"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" s="2"/>
+      <c r="B36" s="2"/>
+      <c r="C36" s="3"/>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" s="2"/>
+      <c r="B37" s="2"/>
+      <c r="C37" s="3"/>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" s="2"/>
+      <c r="B38" s="2"/>
+      <c r="C38" s="3"/>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" s="2"/>
+      <c r="B39" s="2"/>
+      <c r="C39" s="3"/>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40" s="2"/>
+      <c r="B40" s="2"/>
+      <c r="C40" s="3"/>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41" s="2"/>
+      <c r="B41" s="2"/>
+      <c r="C41" s="3"/>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42" s="2"/>
+      <c r="B42" s="2"/>
+      <c r="C42" s="3"/>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43" s="2"/>
+      <c r="B43" s="2"/>
+      <c r="C43" s="3"/>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44" s="2"/>
+      <c r="B44" s="2"/>
+      <c r="C44" s="3"/>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A45" s="2"/>
+      <c r="B45" s="2"/>
+      <c r="C45" s="3"/>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A46" s="2"/>
+      <c r="B46" s="2"/>
+      <c r="C46" s="3"/>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A47" s="2"/>
+      <c r="B47" s="2"/>
+      <c r="C47" s="3"/>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A48" s="2"/>
+      <c r="B48" s="2"/>
+      <c r="C48" s="3"/>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A49" s="2"/>
+      <c r="B49" s="2"/>
+      <c r="C49" s="3"/>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A50" s="2"/>
+      <c r="B50" s="2"/>
+      <c r="C50" s="3"/>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A51" s="2"/>
+      <c r="B51" s="2"/>
+      <c r="C51" s="3"/>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A52" s="2"/>
+      <c r="B52" s="2"/>
+      <c r="C52" s="3"/>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A53" s="2"/>
+      <c r="B53" s="2"/>
+      <c r="C53" s="3"/>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A54" s="2"/>
+      <c r="B54" s="2"/>
+      <c r="C54" s="3"/>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A55" s="2"/>
+      <c r="B55" s="2"/>
+      <c r="C55" s="3"/>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A56" s="2"/>
+      <c r="B56" s="2"/>
+      <c r="C56" s="3"/>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A57" s="2"/>
+      <c r="B57" s="2"/>
+      <c r="C57" s="3"/>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A58" s="2"/>
+      <c r="B58" s="2"/>
+      <c r="C58" s="3"/>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A59" s="2"/>
+      <c r="B59" s="2"/>
+      <c r="C59" s="3"/>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A60" s="2"/>
+      <c r="B60" s="2"/>
+      <c r="C60" s="3"/>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A61" s="2"/>
+      <c r="B61" s="2"/>
+      <c r="C61" s="3"/>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A62" s="2"/>
+      <c r="B62" s="2"/>
+      <c r="C62" s="3"/>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A63" s="2"/>
+      <c r="B63" s="2"/>
+      <c r="C63" s="3"/>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A64" s="2"/>
+      <c r="B64" s="2"/>
+      <c r="C64" s="3"/>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A65" s="2"/>
+      <c r="B65" s="2"/>
+      <c r="C65" s="3"/>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A66" s="2"/>
+      <c r="B66" s="2"/>
+      <c r="C66" s="3"/>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A67" s="2"/>
+      <c r="B67" s="2"/>
+      <c r="C67" s="3"/>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A68" s="2"/>
+      <c r="B68" s="2"/>
+      <c r="C68" s="3"/>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A69" s="2"/>
+      <c r="B69" s="2"/>
+      <c r="C69" s="3"/>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A70" s="2"/>
+      <c r="B70" s="2"/>
+      <c r="C70" s="3"/>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A71" s="2"/>
+      <c r="B71" s="2"/>
+      <c r="C71" s="3"/>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A72" s="2"/>
+      <c r="B72" s="2"/>
+      <c r="C72" s="3"/>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A73" s="2"/>
+      <c r="B73" s="2"/>
+      <c r="C73" s="3"/>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A74" s="2"/>
+      <c r="B74" s="2"/>
+      <c r="C74" s="3"/>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A75" s="2"/>
+      <c r="B75" s="2"/>
+      <c r="C75" s="3"/>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A76" s="2"/>
+      <c r="B76" s="2"/>
+      <c r="C76" s="3"/>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A77" s="2"/>
+      <c r="B77" s="2"/>
+      <c r="C77" s="3"/>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A78" s="2"/>
+      <c r="B78" s="2"/>
+      <c r="C78" s="3"/>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A79" s="2"/>
+      <c r="B79" s="2"/>
+      <c r="C79" s="3"/>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A80" s="2"/>
+      <c r="B80" s="2"/>
+      <c r="C80" s="3"/>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A81" s="2"/>
+      <c r="B81" s="2"/>
+      <c r="C81" s="3"/>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A82" s="2"/>
+      <c r="B82" s="2"/>
+      <c r="C82" s="3"/>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A83" s="2"/>
+      <c r="B83" s="2"/>
+      <c r="C83" s="3"/>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A84" s="2"/>
+      <c r="B84" s="2"/>
+      <c r="C84" s="3"/>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A85" s="2"/>
+      <c r="B85" s="2"/>
+      <c r="C85" s="3"/>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A86" s="2"/>
+      <c r="B86" s="2"/>
+      <c r="C86" s="3"/>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A87" s="2"/>
+      <c r="B87" s="2"/>
+      <c r="C87" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -572,9 +916,6 @@
     <hyperlink ref="B5" r:id="rId3" xr:uid="{D291E8B8-B45B-4774-A4CB-F99600798759}"/>
     <hyperlink ref="B6" r:id="rId4" xr:uid="{316C126E-1C3C-422B-A6CD-D65DE87A9386}"/>
     <hyperlink ref="B4" r:id="rId5" xr:uid="{673F7DAB-FDB5-4CC0-80B9-B05BEB31F6BB}"/>
-    <hyperlink ref="B7" r:id="rId6" xr:uid="{2928EF62-0B49-4B49-9438-6A3A72BD1AC2}"/>
-    <hyperlink ref="B8" r:id="rId7" xr:uid="{D149DE3E-48BD-4418-ABE1-F70662320271}"/>
-    <hyperlink ref="B9" r:id="rId8" xr:uid="{1FDE197F-6542-4E21-9541-D39C46006F80}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>